<commit_message>
leitura de imagem de QRcode com sucesso para nfe-sp
</commit_message>
<xml_diff>
--- a/notas_fiscais.xlsx
+++ b/notas_fiscais.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -515,6 +515,46 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>NOME NÃO ENCONTRADO</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>CNPJ NÃO ENCONTRADO</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2025-09-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>RESTAURANTE DOM PEDRO LTDA</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>03.031.196/0001-70</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>81.90000000000001</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2025-09-02</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>